<commit_message>
resultats LLM only approach
</commit_message>
<xml_diff>
--- a/data/dataset.xlsx
+++ b/data/dataset.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\victo\Documents\LLM\mva-llm-project\data\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{4D72CB04-4836-47AC-85A6-96F06018F4D3}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{702F1D5A-76FD-4DAB-A3BA-F4897154BBA9}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="11424" yWindow="0" windowWidth="11712" windowHeight="13776" activeTab="1" xr2:uid="{09A1F300-4FE8-4DB4-A827-5072DD512702}"/>
+    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="13896" activeTab="1" xr2:uid="{09A1F300-4FE8-4DB4-A827-5072DD512702}"/>
   </bookViews>
   <sheets>
     <sheet name="data" sheetId="1" r:id="rId1"/>
@@ -37,7 +37,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="479" uniqueCount="80">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="581" uniqueCount="85">
   <si>
     <t>PatientID</t>
   </si>
@@ -258,15 +258,6 @@
     <t>LLM only approach</t>
   </si>
   <si>
-    <t>Mistral</t>
-  </si>
-  <si>
-    <t>DeepSeek</t>
-  </si>
-  <si>
-    <t>Llama</t>
-  </si>
-  <si>
     <t>-</t>
   </si>
   <si>
@@ -277,13 +268,37 @@
   </si>
   <si>
     <t>BPD1 or RDD</t>
+  </si>
+  <si>
+    <t xml:space="preserve">- </t>
+  </si>
+  <si>
+    <t>Llama 7b</t>
+  </si>
+  <si>
+    <t>DeepSeek 8b</t>
+  </si>
+  <si>
+    <t>Mistral 7b</t>
+  </si>
+  <si>
+    <t>Unclear</t>
+  </si>
+  <si>
+    <t>(13+3)/30</t>
+  </si>
+  <si>
+    <t>23/30</t>
+  </si>
+  <si>
+    <t>18/30</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="5" x14ac:knownFonts="1">
+  <fonts count="6" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -318,6 +333,14 @@
       <family val="2"/>
       <scheme val="minor"/>
     </font>
+    <font>
+      <b/>
+      <sz val="11"/>
+      <color theme="1"/>
+      <name val="Aptos Narrow"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
   </fonts>
   <fills count="3">
     <fill>
@@ -333,7 +356,7 @@
       </patternFill>
     </fill>
   </fills>
-  <borders count="4">
+  <borders count="7">
     <border>
       <left/>
       <right/>
@@ -370,11 +393,46 @@
       <bottom/>
       <diagonal/>
     </border>
+    <border>
+      <left/>
+      <right style="thin">
+        <color indexed="64"/>
+      </right>
+      <top/>
+      <bottom style="thin">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color indexed="64"/>
+      </left>
+      <right style="thin">
+        <color indexed="64"/>
+      </right>
+      <top/>
+      <bottom style="thin">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right style="thin">
+        <color indexed="64"/>
+      </right>
+      <top style="thin">
+        <color indexed="64"/>
+      </top>
+      <bottom/>
+      <diagonal/>
+    </border>
   </borders>
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="16">
+  <cellXfs count="31">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" quotePrefix="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
@@ -398,18 +456,6 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="3" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="2" borderId="3" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="2" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
@@ -419,102 +465,68 @@
     <xf numFmtId="0" fontId="4" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="3" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="1" xfId="0" quotePrefix="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" quotePrefix="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="1" xfId="0" quotePrefix="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="4" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="5" xfId="0" quotePrefix="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="5" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="4" xfId="0" quotePrefix="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="6" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" quotePrefix="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="2" xfId="0" quotePrefix="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" xfId="0" quotePrefix="1" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
-  <dxfs count="18">
-    <dxf>
-      <font>
-        <color rgb="FFFFC000"/>
-      </font>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FFFF0000"/>
-      </font>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF00B050"/>
-      </font>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FFFFC000"/>
-      </font>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FFFF0000"/>
-      </font>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF00B050"/>
-      </font>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FFFFC000"/>
-      </font>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FFFF0000"/>
-      </font>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF00B050"/>
-      </font>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FFFF0000"/>
-      </font>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF00B050"/>
-      </font>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF00B050"/>
-      </font>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FFFF0000"/>
-      </font>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF00B050"/>
-      </font>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF00B050"/>
-      </font>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF00B050"/>
-      </font>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF00B050"/>
-      </font>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF00B050"/>
-      </font>
-    </dxf>
-  </dxfs>
+  <dxfs count="0"/>
   <tableStyles count="0" defaultTableStyle="TableStyleMedium2" defaultPivotStyle="PivotStyleLight16"/>
   <extLst>
     <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{EB79DEF2-80B8-43e5-95BD-54CBDDF9020C}">
@@ -846,7 +858,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{803366E8-C0BB-464F-8A85-EFB5E956E12C}">
   <dimension ref="A1:G140"/>
   <sheetViews>
-    <sheetView topLeftCell="A31" workbookViewId="0">
+    <sheetView topLeftCell="A103" workbookViewId="0">
       <selection activeCell="C1" sqref="C1"/>
     </sheetView>
   </sheetViews>
@@ -3009,10 +3021,10 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{43CD8D9A-081A-4242-8FC7-DB2AE51F4615}">
-  <dimension ref="A1:G12"/>
+  <dimension ref="A1:G34"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="C5" sqref="C5"/>
+      <selection activeCell="I28" sqref="I28"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -3030,23 +3042,23 @@
       <c r="B1" s="5" t="s">
         <v>71</v>
       </c>
-      <c r="C1" s="10" t="s">
+      <c r="C1" s="12" t="s">
         <v>72</v>
       </c>
-      <c r="D1" s="11"/>
-      <c r="E1" s="12"/>
+      <c r="D1" s="13"/>
+      <c r="E1" s="14"/>
     </row>
     <row r="2" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A2" s="4"/>
       <c r="B2" s="6"/>
       <c r="C2" s="8" t="s">
-        <v>73</v>
-      </c>
-      <c r="D2" s="9" t="s">
-        <v>74</v>
+        <v>80</v>
+      </c>
+      <c r="D2" s="2" t="s">
+        <v>79</v>
       </c>
       <c r="E2" s="4" t="s">
-        <v>75</v>
+        <v>78</v>
       </c>
     </row>
     <row r="3" spans="1:5" x14ac:dyDescent="0.3">
@@ -3056,13 +3068,15 @@
       <c r="B3" s="6" t="s">
         <v>5</v>
       </c>
-      <c r="C3" s="14" t="s">
+      <c r="C3" s="10" t="s">
         <v>16</v>
       </c>
-      <c r="D3" s="9" t="s">
-        <v>5</v>
-      </c>
-      <c r="E3" s="4"/>
+      <c r="D3" s="16" t="s">
+        <v>5</v>
+      </c>
+      <c r="E3" s="16" t="s">
+        <v>5</v>
+      </c>
     </row>
     <row r="4" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A4" s="4">
@@ -3071,11 +3085,15 @@
       <c r="B4" s="6" t="s">
         <v>16</v>
       </c>
-      <c r="C4" s="13" t="s">
+      <c r="C4" s="9" t="s">
         <v>16</v>
       </c>
-      <c r="D4" s="9"/>
-      <c r="E4" s="4"/>
+      <c r="D4" s="15" t="s">
+        <v>39</v>
+      </c>
+      <c r="E4" s="15" t="s">
+        <v>39</v>
+      </c>
     </row>
     <row r="5" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A5" s="4">
@@ -3084,11 +3102,15 @@
       <c r="B5" s="6" t="s">
         <v>23</v>
       </c>
-      <c r="C5" s="13" t="s">
-        <v>23</v>
-      </c>
-      <c r="D5" s="9"/>
-      <c r="E5" s="4"/>
+      <c r="C5" s="9" t="s">
+        <v>23</v>
+      </c>
+      <c r="D5" s="16" t="s">
+        <v>23</v>
+      </c>
+      <c r="E5" s="16" t="s">
+        <v>23</v>
+      </c>
     </row>
     <row r="6" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A6" s="4">
@@ -3097,11 +3119,15 @@
       <c r="B6" s="6" t="s">
         <v>5</v>
       </c>
-      <c r="C6" s="13" t="s">
-        <v>39</v>
-      </c>
-      <c r="D6" s="9"/>
-      <c r="E6" s="4"/>
+      <c r="C6" s="9" t="s">
+        <v>39</v>
+      </c>
+      <c r="D6" s="16" t="s">
+        <v>5</v>
+      </c>
+      <c r="E6" s="16" t="s">
+        <v>5</v>
+      </c>
     </row>
     <row r="7" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A7" s="4">
@@ -3110,11 +3136,15 @@
       <c r="B7" s="6" t="s">
         <v>23</v>
       </c>
-      <c r="C7" s="14" t="s">
-        <v>39</v>
-      </c>
-      <c r="D7" s="9"/>
-      <c r="E7" s="4"/>
+      <c r="C7" s="15" t="s">
+        <v>39</v>
+      </c>
+      <c r="D7" s="17" t="s">
+        <v>77</v>
+      </c>
+      <c r="E7" s="15" t="s">
+        <v>5</v>
+      </c>
     </row>
     <row r="8" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A8" s="4">
@@ -3123,11 +3153,15 @@
       <c r="B8" s="6" t="s">
         <v>5</v>
       </c>
-      <c r="C8" s="15" t="s">
-        <v>77</v>
-      </c>
-      <c r="D8" s="9"/>
-      <c r="E8" s="4"/>
+      <c r="C8" s="11" t="s">
+        <v>74</v>
+      </c>
+      <c r="D8" s="16" t="s">
+        <v>5</v>
+      </c>
+      <c r="E8" s="16" t="s">
+        <v>5</v>
+      </c>
     </row>
     <row r="9" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A9" s="4">
@@ -3136,11 +3170,15 @@
       <c r="B9" s="6" t="s">
         <v>23</v>
       </c>
-      <c r="C9" s="14" t="s">
-        <v>78</v>
-      </c>
-      <c r="D9" s="9"/>
-      <c r="E9" s="4"/>
+      <c r="C9" s="10" t="s">
+        <v>75</v>
+      </c>
+      <c r="D9" s="16" t="s">
+        <v>23</v>
+      </c>
+      <c r="E9" s="16" t="s">
+        <v>23</v>
+      </c>
     </row>
     <row r="10" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A10" s="4">
@@ -3149,11 +3187,15 @@
       <c r="B10" s="6" t="s">
         <v>39</v>
       </c>
-      <c r="C10" s="14" t="s">
-        <v>79</v>
-      </c>
-      <c r="D10" s="9"/>
-      <c r="E10" s="4"/>
+      <c r="C10" s="10" t="s">
+        <v>76</v>
+      </c>
+      <c r="D10" s="16" t="s">
+        <v>39</v>
+      </c>
+      <c r="E10" s="26" t="s">
+        <v>5</v>
+      </c>
     </row>
     <row r="11" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A11" s="4">
@@ -3162,24 +3204,387 @@
       <c r="B11" s="6" t="s">
         <v>39</v>
       </c>
-      <c r="C11" s="14" t="s">
+      <c r="C11" s="10" t="s">
         <v>16</v>
       </c>
-      <c r="D11" s="9"/>
-      <c r="E11" s="4"/>
+      <c r="D11" s="16" t="s">
+        <v>39</v>
+      </c>
+      <c r="E11" s="25" t="s">
+        <v>39</v>
+      </c>
     </row>
     <row r="12" spans="1:5" x14ac:dyDescent="0.3">
-      <c r="A12" s="4">
+      <c r="A12" s="21">
         <v>10</v>
       </c>
-      <c r="B12" s="7" t="s">
-        <v>76</v>
-      </c>
-      <c r="C12" s="14" t="s">
-        <v>39</v>
-      </c>
-      <c r="D12" s="9"/>
-      <c r="E12" s="4"/>
+      <c r="B12" s="22" t="s">
+        <v>73</v>
+      </c>
+      <c r="C12" s="23" t="s">
+        <v>39</v>
+      </c>
+      <c r="D12" s="24" t="s">
+        <v>77</v>
+      </c>
+      <c r="E12" s="24" t="s">
+        <v>77</v>
+      </c>
+    </row>
+    <row r="13" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A13" s="27">
+        <v>11</v>
+      </c>
+      <c r="B13" s="7" t="s">
+        <v>73</v>
+      </c>
+      <c r="C13" s="10" t="s">
+        <v>5</v>
+      </c>
+      <c r="D13" s="7" t="s">
+        <v>77</v>
+      </c>
+      <c r="E13" s="18" t="s">
+        <v>77</v>
+      </c>
+    </row>
+    <row r="14" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A14" s="4">
+        <v>12</v>
+      </c>
+      <c r="B14" s="6" t="s">
+        <v>23</v>
+      </c>
+      <c r="C14" s="16" t="s">
+        <v>23</v>
+      </c>
+      <c r="D14" s="29" t="s">
+        <v>77</v>
+      </c>
+      <c r="E14" s="26" t="s">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="15" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A15" s="4">
+        <v>13</v>
+      </c>
+      <c r="B15" s="6" t="s">
+        <v>23</v>
+      </c>
+      <c r="C15" s="16" t="s">
+        <v>23</v>
+      </c>
+      <c r="D15" s="16" t="s">
+        <v>23</v>
+      </c>
+      <c r="E15" s="25" t="s">
+        <v>23</v>
+      </c>
+    </row>
+    <row r="16" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A16" s="4">
+        <v>14</v>
+      </c>
+      <c r="B16" s="6" t="s">
+        <v>23</v>
+      </c>
+      <c r="C16" s="16" t="s">
+        <v>23</v>
+      </c>
+      <c r="D16" s="16" t="s">
+        <v>23</v>
+      </c>
+      <c r="E16" s="26" t="s">
+        <v>39</v>
+      </c>
+    </row>
+    <row r="17" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A17" s="4">
+        <v>15</v>
+      </c>
+      <c r="B17" s="6" t="s">
+        <v>5</v>
+      </c>
+      <c r="C17" s="15" t="s">
+        <v>23</v>
+      </c>
+      <c r="D17" s="15" t="s">
+        <v>23</v>
+      </c>
+      <c r="E17" s="25" t="s">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="18" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A18" s="4">
+        <v>16</v>
+      </c>
+      <c r="B18" s="6" t="s">
+        <v>5</v>
+      </c>
+      <c r="C18" s="26" t="s">
+        <v>16</v>
+      </c>
+      <c r="D18" s="16" t="s">
+        <v>5</v>
+      </c>
+      <c r="E18" s="25" t="s">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="19" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A19" s="4">
+        <v>17</v>
+      </c>
+      <c r="B19" s="6" t="s">
+        <v>23</v>
+      </c>
+      <c r="C19" s="25" t="s">
+        <v>23</v>
+      </c>
+      <c r="D19" s="16" t="s">
+        <v>23</v>
+      </c>
+      <c r="E19" s="25" t="s">
+        <v>23</v>
+      </c>
+    </row>
+    <row r="20" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A20" s="4">
+        <v>18</v>
+      </c>
+      <c r="B20" s="6" t="s">
+        <v>16</v>
+      </c>
+      <c r="C20" s="25" t="s">
+        <v>16</v>
+      </c>
+      <c r="D20" s="16" t="s">
+        <v>16</v>
+      </c>
+      <c r="E20" s="26" t="s">
+        <v>23</v>
+      </c>
+    </row>
+    <row r="21" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A21" s="4">
+        <v>19</v>
+      </c>
+      <c r="B21" s="6" t="s">
+        <v>5</v>
+      </c>
+      <c r="C21" s="25" t="s">
+        <v>5</v>
+      </c>
+      <c r="D21" s="16" t="s">
+        <v>5</v>
+      </c>
+      <c r="E21" s="25" t="s">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="22" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A22" s="4">
+        <v>20</v>
+      </c>
+      <c r="B22" s="6" t="s">
+        <v>39</v>
+      </c>
+      <c r="C22" s="25" t="s">
+        <v>39</v>
+      </c>
+      <c r="D22" s="16" t="s">
+        <v>39</v>
+      </c>
+      <c r="E22" s="17" t="s">
+        <v>73</v>
+      </c>
+    </row>
+    <row r="23" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A23" s="4">
+        <v>21</v>
+      </c>
+      <c r="B23" s="6" t="s">
+        <v>23</v>
+      </c>
+      <c r="C23" s="28" t="s">
+        <v>16</v>
+      </c>
+      <c r="D23" s="16" t="s">
+        <v>23</v>
+      </c>
+      <c r="E23" s="26" t="s">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="24" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A24" s="4">
+        <v>22</v>
+      </c>
+      <c r="B24" s="6" t="s">
+        <v>23</v>
+      </c>
+      <c r="C24" s="25" t="s">
+        <v>23</v>
+      </c>
+      <c r="D24" s="16" t="s">
+        <v>23</v>
+      </c>
+      <c r="E24" s="26" t="s">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="25" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A25" s="4">
+        <v>23</v>
+      </c>
+      <c r="B25" s="6" t="s">
+        <v>5</v>
+      </c>
+      <c r="C25" s="26" t="s">
+        <v>23</v>
+      </c>
+      <c r="D25" s="15" t="s">
+        <v>39</v>
+      </c>
+      <c r="E25" s="25" t="s">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="26" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A26" s="4">
+        <v>24</v>
+      </c>
+      <c r="B26" s="7" t="s">
+        <v>73</v>
+      </c>
+      <c r="C26" s="18" t="s">
+        <v>73</v>
+      </c>
+      <c r="D26" s="7" t="s">
+        <v>73</v>
+      </c>
+      <c r="E26" s="19" t="s">
+        <v>73</v>
+      </c>
+    </row>
+    <row r="27" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A27" s="4">
+        <v>25</v>
+      </c>
+      <c r="B27" s="6" t="s">
+        <v>16</v>
+      </c>
+      <c r="C27" s="11" t="s">
+        <v>75</v>
+      </c>
+      <c r="D27" s="15" t="s">
+        <v>39</v>
+      </c>
+      <c r="E27" s="26" t="s">
+        <v>39</v>
+      </c>
+    </row>
+    <row r="28" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A28" s="4">
+        <v>26</v>
+      </c>
+      <c r="B28" s="6" t="s">
+        <v>5</v>
+      </c>
+      <c r="C28" s="26" t="s">
+        <v>81</v>
+      </c>
+      <c r="D28" s="16" t="s">
+        <v>5</v>
+      </c>
+      <c r="E28" s="25" t="s">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="29" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A29" s="4">
+        <v>27</v>
+      </c>
+      <c r="B29" s="6" t="s">
+        <v>39</v>
+      </c>
+      <c r="C29" s="11" t="s">
+        <v>75</v>
+      </c>
+      <c r="D29" s="16" t="s">
+        <v>39</v>
+      </c>
+      <c r="E29" s="26" t="s">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="30" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A30" s="4">
+        <v>28</v>
+      </c>
+      <c r="B30" s="6" t="s">
+        <v>39</v>
+      </c>
+      <c r="C30" s="28" t="s">
+        <v>16</v>
+      </c>
+      <c r="D30" s="6" t="s">
+        <v>39</v>
+      </c>
+      <c r="E30" s="25" t="s">
+        <v>39</v>
+      </c>
+    </row>
+    <row r="31" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A31" s="4">
+        <v>29</v>
+      </c>
+      <c r="B31" s="6" t="s">
+        <v>16</v>
+      </c>
+      <c r="C31" s="25" t="s">
+        <v>16</v>
+      </c>
+      <c r="D31" s="15" t="s">
+        <v>39</v>
+      </c>
+      <c r="E31" s="26" t="s">
+        <v>39</v>
+      </c>
+    </row>
+    <row r="32" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A32" s="4">
+        <v>30</v>
+      </c>
+      <c r="B32" s="7" t="s">
+        <v>73</v>
+      </c>
+      <c r="C32" s="26" t="s">
+        <v>23</v>
+      </c>
+      <c r="D32" s="7" t="s">
+        <v>77</v>
+      </c>
+      <c r="E32" s="19" t="s">
+        <v>73</v>
+      </c>
+    </row>
+    <row r="33" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A33" s="20"/>
+      <c r="C33" s="30" t="s">
+        <v>82</v>
+      </c>
+      <c r="D33" s="30" t="s">
+        <v>83</v>
+      </c>
+      <c r="E33" s="30" t="s">
+        <v>84</v>
+      </c>
+    </row>
+    <row r="34" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A34" s="20"/>
     </row>
   </sheetData>
   <mergeCells count="1">

</xml_diff>